<commit_message>
DeleteProblemTestFactory tested on 2 lines of data
</commit_message>
<xml_diff>
--- a/resources/DeleteProblemTestData.xlsx
+++ b/resources/DeleteProblemTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>problemTitle1</t>
   </si>
@@ -79,6 +79,30 @@
   </si>
   <si>
     <t>30.31</t>
+  </si>
+  <si>
+    <t>50.32</t>
+  </si>
+  <si>
+    <t>30.32</t>
+  </si>
+  <si>
+    <t>problemTitle2</t>
+  </si>
+  <si>
+    <t>Сміттєзвалища</t>
+  </si>
+  <si>
+    <t>problemDescription2</t>
+  </si>
+  <si>
+    <t>problemSolution2</t>
+  </si>
+  <si>
+    <t>http://i.imgur.com/1K6AdCH.jpg</t>
+  </si>
+  <si>
+    <t>imageComment1</t>
   </si>
 </sst>
 </file>
@@ -423,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -512,8 +536,46 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>